<commit_message>
OpenGL code ALMOST ready!
</commit_message>
<xml_diff>
--- a/Day2Day/Classes_calendar.xlsx
+++ b/Day2Day/Classes_calendar.xlsx
@@ -1,17 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\z_FS\3111_3D\2022\INFO3111S22\Day2Day\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7C483F4-CCBC-4594-B9F0-DD22E5B4AC41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650"/>
+    <workbookView xWindow="15705" yWindow="2190" windowWidth="10230" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="125725"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -111,9 +117,6 @@
     <t>Final Exam</t>
   </si>
   <si>
-    <t>Friday, July 13th, 2022</t>
-  </si>
-  <si>
     <t>TBD</t>
   </si>
   <si>
@@ -169,13 +172,16 @@
   </si>
   <si>
     <t>INFO-3111 Summer 2022 : Feeney</t>
+  </si>
+  <si>
+    <t>Friday, July 15th, 2022</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -487,31 +493,33 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4:C14"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.453125" customWidth="1"/>
-    <col min="2" max="2" width="25.26953125" customWidth="1"/>
-    <col min="3" max="3" width="17.1796875" customWidth="1"/>
+    <col min="1" max="1" width="10.42578125" customWidth="1"/>
+    <col min="2" max="2" width="25.28515625" customWidth="1"/>
+    <col min="3" max="3" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -519,7 +527,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -527,10 +535,10 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -538,10 +546,10 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -549,10 +557,10 @@
         <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -560,10 +568,10 @@
         <v>9</v>
       </c>
       <c r="C9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -571,10 +579,10 @@
         <v>19</v>
       </c>
       <c r="C10" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -582,10 +590,10 @@
         <v>20</v>
       </c>
       <c r="C12" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -593,23 +601,23 @@
         <v>21</v>
       </c>
       <c r="C13" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B16" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>13</v>
       </c>
@@ -617,7 +625,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>14</v>
       </c>
@@ -625,10 +633,10 @@
         <v>23</v>
       </c>
       <c r="C19" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>15</v>
       </c>
@@ -636,10 +644,10 @@
         <v>24</v>
       </c>
       <c r="C21" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>16</v>
       </c>
@@ -647,10 +655,10 @@
         <v>25</v>
       </c>
       <c r="C22" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>17</v>
       </c>
@@ -658,10 +666,10 @@
         <v>26</v>
       </c>
       <c r="C24" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>18</v>
       </c>
@@ -669,35 +677,35 @@
         <v>27</v>
       </c>
       <c r="C25" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B28" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
-      <c r="A30" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3">
-      <c r="B31" t="s">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
         <v>32</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3">
-      <c r="B32" t="s">
-        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>